<commit_message>
statistics output and CPUE output
</commit_message>
<xml_diff>
--- a/FishLandings/output/statistics.xlsx
+++ b/FishLandings/output/statistics.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/Kenya_SamakiSalama/FishLandings/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4869397-5AAB-034B-91FC-0D7E47FDCEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC136B6-444C-8B49-AE38-FBD9A48C274E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="460" windowWidth="28020" windowHeight="19700" xr2:uid="{5FDCE57C-5292-474E-8C9B-DC97E3A3B8AB}"/>
+    <workbookView xWindow="5580" yWindow="460" windowWidth="28020" windowHeight="19700" activeTab="1" xr2:uid="{5FDCE57C-5292-474E-8C9B-DC97E3A3B8AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Fig1 stats" sheetId="1" r:id="rId1"/>
+    <sheet name="Table 1 Methods" sheetId="2" r:id="rId1"/>
+    <sheet name="Table 2 CPUE Results" sheetId="3" r:id="rId2"/>
+    <sheet name="Supp Table 1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
   <si>
     <t>Dependent Variable</t>
   </si>
@@ -75,6 +77,165 @@
   </si>
   <si>
     <t xml:space="preserve">Reported Yield (Biomass; kg per trap) </t>
+  </si>
+  <si>
+    <t>Acanthurus dussumieri</t>
+  </si>
+  <si>
+    <t>Acanthurus triostegus</t>
+  </si>
+  <si>
+    <t>Acanthurus xanthopterus</t>
+  </si>
+  <si>
+    <t>Cephalopholis argus</t>
+  </si>
+  <si>
+    <t>Gerres oyena</t>
+  </si>
+  <si>
+    <t>Hipposcarus harid</t>
+  </si>
+  <si>
+    <t>Leptoscarus vaigiensis</t>
+  </si>
+  <si>
+    <t>Lethrinus conchyliatus</t>
+  </si>
+  <si>
+    <t>Lethrinus harak</t>
+  </si>
+  <si>
+    <t>Lethrinus nebulosus</t>
+  </si>
+  <si>
+    <t>Lutjanus fulviflamma</t>
+  </si>
+  <si>
+    <t>Monotaxis grandoculis</t>
+  </si>
+  <si>
+    <t>Mulloidichthys flavolineatus</t>
+  </si>
+  <si>
+    <t>Naso annulatus</t>
+  </si>
+  <si>
+    <t>Naso brachycentron</t>
+  </si>
+  <si>
+    <t>Parupeneus heptacanthus</t>
+  </si>
+  <si>
+    <t>Parupeneus macronemus</t>
+  </si>
+  <si>
+    <t>Plectorhinchus gaterinus</t>
+  </si>
+  <si>
+    <t>Plectorhinchus sordidus</t>
+  </si>
+  <si>
+    <t>Plectorhinchus vittatus</t>
+  </si>
+  <si>
+    <t>Sardinella melanura</t>
+  </si>
+  <si>
+    <t>Scarus ghobban</t>
+  </si>
+  <si>
+    <t>Scarus rubroviolaceus</t>
+  </si>
+  <si>
+    <t>Siganus canaliculatus</t>
+  </si>
+  <si>
+    <t>Siganus sutor</t>
+  </si>
+  <si>
+    <t>Trichiurus lepturus</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Acanthuridae</t>
+  </si>
+  <si>
+    <t>Serranidae</t>
+  </si>
+  <si>
+    <t>Gerreidae</t>
+  </si>
+  <si>
+    <t>Scaridae</t>
+  </si>
+  <si>
+    <t>Lethrinidae</t>
+  </si>
+  <si>
+    <t>Lutjanidae</t>
+  </si>
+  <si>
+    <t>Mullidae</t>
+  </si>
+  <si>
+    <t>Haemulidae</t>
+  </si>
+  <si>
+    <t>Clupeidae</t>
+  </si>
+  <si>
+    <t>Siganidae</t>
+  </si>
+  <si>
+    <t>Trichiuridae</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Lmax</t>
+  </si>
+  <si>
+    <t>Lm</t>
+  </si>
+  <si>
+    <t>Lopt</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Reported CPUE (n trap-1)</t>
+  </si>
+  <si>
+    <t>Reported Yield (Biomass kg trap-1)</t>
+  </si>
+  <si>
+    <t>Length (cm survey-1)</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Experimental</t>
+  </si>
+  <si>
+    <t>Mean +/- SE</t>
   </si>
 </sst>
 </file>
@@ -86,7 +247,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -121,6 +282,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -136,7 +303,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -164,12 +331,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -203,6 +382,49 @@
     </xf>
     <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,194 +739,1107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE2254E-2433-4745-91B6-A5A22A311AC2}">
-  <dimension ref="B2:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C761741E-3895-7841-892D-BAC3B98047AF}">
+  <dimension ref="B2:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="41.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="7"/>
-    <col min="4" max="4" width="10.83203125" style="7" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="7"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="28.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="18">
+        <v>54</v>
+      </c>
+      <c r="E3" s="18">
+        <v>23.2</v>
+      </c>
+      <c r="F3" s="18">
+        <v>25.2</v>
+      </c>
+      <c r="G3" s="23">
+        <v>4.2560000000000001E-2</v>
+      </c>
+      <c r="H3" s="24">
+        <v>2.8679999999999999</v>
+      </c>
+      <c r="I3" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="18">
+        <v>27</v>
+      </c>
+      <c r="E4" s="18">
+        <v>12.3</v>
+      </c>
+      <c r="F4" s="18">
+        <v>12.2</v>
+      </c>
+      <c r="G4" s="23">
+        <v>3.61E-2</v>
+      </c>
+      <c r="H4" s="24">
+        <v>3.13</v>
+      </c>
+      <c r="I4" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="18">
+        <v>70</v>
+      </c>
+      <c r="E5" s="18">
+        <v>35.5</v>
+      </c>
+      <c r="F5" s="18">
+        <v>41.2</v>
+      </c>
+      <c r="G5" s="23">
+        <v>2.673E-2</v>
+      </c>
+      <c r="H5" s="24">
+        <v>2.984</v>
+      </c>
+      <c r="I5" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="18">
+        <v>60</v>
+      </c>
+      <c r="E6" s="18">
+        <v>34.1</v>
+      </c>
+      <c r="F6" s="18">
+        <v>39.4</v>
+      </c>
+      <c r="G6" s="23">
+        <v>1.17E-2</v>
+      </c>
+      <c r="H6" s="24">
+        <v>3.14</v>
+      </c>
+      <c r="I6" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="18">
+        <v>30</v>
+      </c>
+      <c r="E7" s="18">
+        <v>18.5</v>
+      </c>
+      <c r="F7" s="18">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="G7" s="23">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="H7" s="24">
+        <v>2.96</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="18">
+        <v>75</v>
+      </c>
+      <c r="E8" s="18">
+        <v>30</v>
+      </c>
+      <c r="F8" s="18">
+        <v>34</v>
+      </c>
+      <c r="G8" s="23">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="H8" s="24">
+        <v>2.91</v>
+      </c>
+      <c r="I8" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="18">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="E9" s="18">
+        <v>21.3</v>
+      </c>
+      <c r="F9" s="18">
+        <v>22.8</v>
+      </c>
+      <c r="G9" s="23">
+        <v>1.84E-2</v>
+      </c>
+      <c r="H9" s="24">
+        <v>2.94</v>
+      </c>
+      <c r="I9" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="18">
+        <v>76</v>
+      </c>
+      <c r="E10" s="18">
+        <v>42</v>
+      </c>
+      <c r="F10" s="18">
+        <v>50.2</v>
+      </c>
+      <c r="G10" s="23">
+        <v>0</v>
+      </c>
+      <c r="H10" s="24">
+        <v>1.0840000000000001</v>
+      </c>
+      <c r="I10" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="18">
+        <v>50</v>
+      </c>
+      <c r="E11" s="18">
+        <v>23.6</v>
+      </c>
+      <c r="F11" s="18">
+        <v>25.8</v>
+      </c>
+      <c r="G11" s="23">
+        <v>1.7010000000000001E-2</v>
+      </c>
+      <c r="H11" s="24">
+        <v>3.0419999999999998</v>
+      </c>
+      <c r="I11" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="18">
+        <v>87</v>
+      </c>
+      <c r="E12" s="18">
+        <v>37.4</v>
+      </c>
+      <c r="F12" s="18">
+        <v>43.9</v>
+      </c>
+      <c r="G12" s="23">
+        <v>1.8710000000000001E-2</v>
+      </c>
+      <c r="H12" s="24">
+        <v>2.996</v>
+      </c>
+      <c r="I12" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="18">
+        <v>35</v>
+      </c>
+      <c r="E13" s="18">
+        <v>13.6</v>
+      </c>
+      <c r="F13" s="18">
+        <v>14</v>
+      </c>
+      <c r="G13" s="23">
+        <v>2.0480000000000002E-2</v>
+      </c>
+      <c r="H13" s="24">
+        <v>2.96</v>
+      </c>
+      <c r="I13" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="18">
+        <v>60</v>
+      </c>
+      <c r="E14" s="18">
+        <v>34.1</v>
+      </c>
+      <c r="F14" s="18">
+        <v>39.4</v>
+      </c>
+      <c r="G14" s="23">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="H14" s="24">
+        <v>2.84</v>
+      </c>
+      <c r="I14" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="18">
+        <v>43</v>
+      </c>
+      <c r="E15" s="18">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="F15" s="18">
+        <v>21</v>
+      </c>
+      <c r="G15" s="23">
+        <v>1.38E-2</v>
+      </c>
+      <c r="H15" s="24">
+        <v>3.05</v>
+      </c>
+      <c r="I15" s="18">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="18">
+        <v>100</v>
+      </c>
+      <c r="E16" s="18">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="F16" s="18">
+        <v>46.4</v>
+      </c>
+      <c r="G16" s="23">
+        <v>5.1029999999999999E-2</v>
+      </c>
+      <c r="H16" s="24">
+        <v>2.7149999999999999</v>
+      </c>
+      <c r="I16" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="18">
+        <v>90</v>
+      </c>
+      <c r="E17" s="18">
+        <v>48.8</v>
+      </c>
+      <c r="F17" s="18">
+        <v>59.7</v>
+      </c>
+      <c r="G17" s="23">
+        <v>1.89E-2</v>
+      </c>
+      <c r="H17" s="24">
+        <v>2.99</v>
+      </c>
+      <c r="I17" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="18">
+        <v>36</v>
+      </c>
+      <c r="E18" s="18">
+        <v>17.5</v>
+      </c>
+      <c r="F18" s="18">
+        <v>18.2</v>
+      </c>
+      <c r="G18" s="23">
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="H18" s="24">
+        <v>3.0779999999999998</v>
+      </c>
+      <c r="I18" s="18">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="18">
+        <v>40</v>
+      </c>
+      <c r="E19" s="18">
+        <v>23.8</v>
+      </c>
+      <c r="F19" s="18">
+        <v>26</v>
+      </c>
+      <c r="G19" s="23">
+        <v>5.4599999999999996E-3</v>
+      </c>
+      <c r="H19" s="24">
+        <v>3.2970000000000002</v>
+      </c>
+      <c r="I19" s="18">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="18">
+        <v>50</v>
+      </c>
+      <c r="E20" s="18">
+        <v>29</v>
+      </c>
+      <c r="F20" s="18">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="G20" s="23">
+        <v>-1.3260000000000001</v>
+      </c>
+      <c r="H20" s="24">
+        <v>0.88</v>
+      </c>
+      <c r="I20" s="18">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="18">
+        <v>60</v>
+      </c>
+      <c r="E21" s="18">
+        <v>34.1</v>
+      </c>
+      <c r="F21" s="18">
+        <v>39.4</v>
+      </c>
+      <c r="G21" s="23">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="H21" s="24">
+        <v>2.75</v>
+      </c>
+      <c r="I21" s="18">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="18">
+        <v>72</v>
+      </c>
+      <c r="E22" s="18">
+        <v>40</v>
+      </c>
+      <c r="F22" s="18">
+        <v>47.4</v>
+      </c>
+      <c r="G22" s="23">
+        <v>-0.78100000000000003</v>
+      </c>
+      <c r="H22" s="24">
+        <v>0.85</v>
+      </c>
+      <c r="I22" s="18">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="18">
+        <v>20.3</v>
+      </c>
+      <c r="E23" s="18">
+        <v>13.5</v>
+      </c>
+      <c r="F23" s="18">
+        <v>13.4</v>
+      </c>
+      <c r="G23" s="23">
+        <v>1.26E-2</v>
+      </c>
+      <c r="H23" s="24">
+        <v>3.04</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="18">
+        <v>75</v>
+      </c>
+      <c r="E24" s="18">
+        <v>41.5</v>
+      </c>
+      <c r="F24" s="18">
+        <v>49.5</v>
+      </c>
+      <c r="G24" s="23">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="H24" s="24">
+        <v>3.0409999999999999</v>
+      </c>
+      <c r="I24" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="18">
+        <v>70</v>
+      </c>
+      <c r="E25" s="18">
+        <v>26.3</v>
+      </c>
+      <c r="F25" s="18">
+        <v>29.2</v>
+      </c>
+      <c r="G25" s="23">
+        <v>1.15E-2</v>
+      </c>
+      <c r="H25" s="24">
+        <v>3.18</v>
+      </c>
+      <c r="I25" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="18">
+        <v>40</v>
+      </c>
+      <c r="E26" s="18">
+        <v>18</v>
+      </c>
+      <c r="F26" s="18">
+        <v>10.6</v>
+      </c>
+      <c r="G26" s="23">
+        <v>1.9900000000000001E-2</v>
+      </c>
+      <c r="H26" s="24">
+        <v>3.1070000000000002</v>
+      </c>
+      <c r="I26" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="18">
+        <v>45</v>
+      </c>
+      <c r="E27" s="18">
+        <v>26</v>
+      </c>
+      <c r="F27" s="18">
+        <v>29.1</v>
+      </c>
+      <c r="G27" s="23">
+        <v>3.2800000000000003E-2</v>
+      </c>
+      <c r="H27" s="24">
+        <v>2.7160000000000002</v>
+      </c>
+      <c r="I27" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="18">
+        <v>234</v>
+      </c>
+      <c r="E28" s="18">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="F28" s="18">
+        <v>108.9</v>
+      </c>
+      <c r="G28" s="23">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="H28" s="24">
+        <v>2.97</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A794481F-4F6D-C649-B0FB-88F056E3A9BA}">
+  <dimension ref="A2:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="1" customWidth="1"/>
+    <col min="7" max="7" width="28" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="26"/>
+      <c r="G2" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="20"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+    </row>
+    <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="19"/>
+      <c r="C11" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="30"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="19"/>
+      <c r="C12" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="20"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="20"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="19"/>
+      <c r="C18" s="20"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="19"/>
+      <c r="C19" s="20"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="19"/>
+      <c r="C20" s="20"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" s="19"/>
+      <c r="C27" s="20"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A14:B14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE2254E-2433-4745-91B6-A5A22A311AC2}">
+  <dimension ref="B2:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="41.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="8"/>
+    <col min="4" max="4" width="10.83203125" style="8" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="8"/>
+    <col min="7" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="10">
         <v>-28.012</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="8">
         <v>1751.4</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="11">
         <v>43.653300000000002</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="11">
         <v>11.58572</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="8">
         <v>-2.4514999999999998</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="8">
         <v>3687.1</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="14">
         <v>1.427E-2</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="11">
         <v>0.83209540000000004</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="11">
         <v>0.79660909999999996</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="8">
         <v>-2.9256000000000002</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="8">
         <v>2959.7</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="14">
         <v>3.4640000000000001E-3</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="11">
         <v>27.14349</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="11">
         <v>26.813230000000001</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="8">
         <v>-6.6608000000000001</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="15">
         <v>5132</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="11">
         <v>166.6003</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="11">
         <v>147.3544</v>
       </c>
     </row>

</xml_diff>